<commit_message>
started editing student responses
</commit_message>
<xml_diff>
--- a/survey_codebooks.xlsx
+++ b/survey_codebooks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t xml:space="preserve">Code</t>
   </si>
@@ -172,6 +172,9 @@
     <t xml:space="preserve">How likely are you to recommend the case studies to others?...25</t>
   </si>
   <si>
+    <t xml:space="preserve">teaching_interests</t>
+  </si>
+  <si>
     <t xml:space="preserve">What specifically brought you to the case studies? (select all that apply)...26</t>
   </si>
   <si>
@@ -274,7 +277,7 @@
     <t xml:space="preserve">student_enjoyment</t>
   </si>
   <si>
-    <t xml:space="preserve">Compared to how you taught similar material previously,  how will did your students seem to enjoy  the case studies?</t>
+    <t xml:space="preserve">Compared to how you taught similar material previously,  how well did your students seem to enjoy  the case studies?</t>
   </si>
   <si>
     <t xml:space="preserve">future_data_use</t>
@@ -1018,34 +1021,34 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11">
@@ -1053,7 +1056,7 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12">
@@ -1066,10 +1069,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14">
@@ -1085,191 +1088,191 @@
         <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B29" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B30" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B33" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B36" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B38" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39">
@@ -1277,47 +1280,47 @@
         <v>18</v>
       </c>
       <c r="B39" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B40" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B41" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B42" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B43" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B44" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1363,7 +1366,7 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5">
@@ -1371,7 +1374,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6">
@@ -1379,7 +1382,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7">
@@ -1387,7 +1390,7 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8">
@@ -1395,7 +1398,7 @@
         <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9">
@@ -1403,7 +1406,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10">
@@ -1411,7 +1414,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11">
@@ -1419,7 +1422,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12">
@@ -1427,7 +1430,7 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13">
@@ -1435,7 +1438,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14">
@@ -1443,7 +1446,7 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15">
@@ -1459,7 +1462,7 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17">
@@ -1475,7 +1478,7 @@
         <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19">
@@ -1483,15 +1486,15 @@
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21">
@@ -1499,7 +1502,7 @@
         <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22">
@@ -1507,7 +1510,7 @@
         <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23">
@@ -1515,7 +1518,7 @@
         <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>